<commit_message>
Removed unused Ej and update publish series,
</commit_message>
<xml_diff>
--- a/governance/reference/SolaceRMValues.xlsx
+++ b/governance/reference/SolaceRMValues.xlsx
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1701,7 +1701,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1755,11 +1755,11 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1881,7 +1881,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1935,7 +1935,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2025,7 +2025,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -2043,7 +2043,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -2061,7 +2061,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -2079,7 +2079,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2097,7 +2097,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -2151,11 +2151,11 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2313,7 +2313,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2331,7 +2331,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2421,11 +2421,11 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2475,7 +2475,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2493,7 +2493,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2511,7 +2511,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2529,7 +2529,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2565,7 +2565,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2601,7 +2601,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2619,7 +2619,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2691,7 +2691,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2709,7 +2709,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2763,7 +2763,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2781,7 +2781,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2799,7 +2799,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2817,7 +2817,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2835,11 +2835,11 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2889,7 +2889,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2997,11 +2997,11 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -3015,11 +3015,11 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -3033,7 +3033,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -3069,7 +3069,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -3105,11 +3105,11 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3141,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -3213,7 +3213,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3231,7 +3231,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3285,7 +3285,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3303,7 +3303,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -3339,7 +3339,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -3357,7 +3357,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -3411,11 +3411,11 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>unrated</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -3447,7 +3447,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
-Adding polygon et al protocols
</commit_message>
<xml_diff>
--- a/governance/reference/SolaceRMValues.xlsx
+++ b/governance/reference/SolaceRMValues.xlsx
@@ -1060,7 +1060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1199,15 +1199,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>alchemix</t>
+          <t>adamant</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
@@ -1217,11 +1217,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>alkemi</t>
+          <t>alchemix</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1235,15 +1235,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>alpha-tokenomics</t>
+          <t>alkemi</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>alpha-v1</t>
+          <t>alpha-tokenomics</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>alpha-v2</t>
+          <t>alpha-v1</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1289,79 +1289,79 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>apy</t>
+          <t>alpha-v2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="15" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>arcx</t>
+          <t>apeswap</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="15" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>armor</t>
+          <t>apy</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="15" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b-protocol</t>
+          <t>arcx</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="15" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>badger</t>
+          <t>armor</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1369,75 +1369,75 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>balancer-v1</t>
+          <t>autofarm</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="15" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>balancer-v2</t>
+          <t>b-protocol</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="15" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>bancor</t>
+          <t>badger</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="15" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>bao</t>
+          <t>balancer-v1</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1447,47 +1447,47 @@
     </row>
     <row r="22">
       <c r="A22" s="15" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>barnbridge</t>
+          <t>balancer-v2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="15" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>barnbridge-smart-yield</t>
+          <t>bancor</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="15" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>bent</t>
+          <t>bao</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1495,53 +1495,53 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="15" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>compound</t>
+          <t>barnbridge</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="15" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>convex</t>
+          <t>barnbridge-smart-yield</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="15" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cream</t>
+          <t>beefy</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1549,39 +1549,39 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="15" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>cryptex</t>
+          <t>beethoven-x</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="15" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>curve</t>
+          <t>belt</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1591,87 +1591,87 @@
     </row>
     <row r="30">
       <c r="A30" s="15" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>defi-swap</t>
+          <t>benqi</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="15" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>defisaver</t>
+          <t>bent</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="15" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>derivadex</t>
+          <t>blizz</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="15" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>deversifi</t>
+          <t>compound</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="15" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>dforce</t>
+          <t>convex</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1681,33 +1681,33 @@
     </row>
     <row r="35">
       <c r="A35" s="15" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>dhedge</t>
+          <t>cream</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="15" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>dodo</t>
+          <t>cryptex</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1717,29 +1717,29 @@
     </row>
     <row r="37">
       <c r="A37" s="15" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>dopex</t>
+          <t>curve</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="15" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>dydx</t>
+          <t>defi-kingdoms</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1753,11 +1753,11 @@
     </row>
     <row r="39">
       <c r="A39" s="15" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>88mph</t>
+          <t>defi-swap</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1765,21 +1765,21 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="15" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>88mph-v3</t>
+          <t>defisaver</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1789,83 +1789,83 @@
     </row>
     <row r="41">
       <c r="A41" s="15" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>element</t>
+          <t>derivadex</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="15" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>fei</t>
+          <t>deversifi</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="15" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>float-protocol</t>
+          <t>dforce</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="15" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>frax</t>
+          <t>dfyn</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="15" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>governor-dao</t>
+          <t>dhedge</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1873,17 +1873,17 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>asset-management</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="15" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>gro</t>
+          <t>dinoswap</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1891,17 +1891,17 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="15" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>harvest</t>
+          <t>dodo</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1909,17 +1909,17 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="15" t="n">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>hegic</t>
+          <t>dopex</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1933,33 +1933,33 @@
     </row>
     <row r="49">
       <c r="A49" s="15" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>hop</t>
+          <t>dydx</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="15" t="n">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>hundred-finance</t>
+          <t>88mph</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1969,11 +1969,11 @@
     </row>
     <row r="51">
       <c r="A51" s="15" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>idle</t>
+          <t>88mph-v3</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1981,107 +1981,107 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="15" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>illuvium</t>
+          <t>element</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="15" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>index-coop</t>
+          <t>eleven-finance</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="15" t="n">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>indexed</t>
+          <t>ellipsis</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="15" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>inverse</t>
+          <t>fei</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>asset-management</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="15" t="n">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>iron</t>
+          <t>float-protocol</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>asset-management</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="15" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>iron-bank</t>
+          <t>frax</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2089,17 +2089,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>asset-management</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="15" t="n">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>keep-network</t>
+          <t>geist</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2107,35 +2107,35 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="15" t="n">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>keeper-dao</t>
+          <t>gmx</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="15" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>klondike</t>
+          <t>governor-dao</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -2143,35 +2143,35 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="15" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>liquity</t>
+          <t>grim</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="15" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>looksrare</t>
+          <t>gro</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -2179,17 +2179,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="15" t="n">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>loopring</t>
+          <t>harvest</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -2197,17 +2197,17 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="15" t="n">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>lyra</t>
+          <t>hector-dao</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2221,33 +2221,33 @@
     </row>
     <row r="65">
       <c r="A65" s="15" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>maple</t>
+          <t>hegic</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="15" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>mirror</t>
+          <t>honeyswap</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2257,29 +2257,29 @@
     </row>
     <row r="67">
       <c r="A67" s="15" t="n">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>mooniswap</t>
+          <t>hop</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="15" t="n">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>mstable</t>
+          <t>hundred-finance</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -2287,35 +2287,35 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="15" t="n">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>nexus-mutual</t>
+          <t>idle</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="15" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>nft20</t>
+          <t>illuvium</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2323,35 +2323,35 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="15" t="n">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>nftx</t>
+          <t>index-coop</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="15" t="n">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>nsure-network</t>
+          <t>indexed</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2365,65 +2365,65 @@
     </row>
     <row r="73">
       <c r="A73" s="15" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>olympus</t>
+          <t>inverse</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="15" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ondo</t>
+          <t>iron</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="15" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>1inch</t>
+          <t>iron-bank</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="15" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>onx</t>
+          <t>jones-dao</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2431,21 +2431,21 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="15" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>opium-network</t>
+          <t>keep-network</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2455,11 +2455,11 @@
     </row>
     <row r="78">
       <c r="A78" s="15" t="n">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>opyn</t>
+          <t>keeper-dao</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2467,21 +2467,21 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="15" t="n">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>origin</t>
+          <t>klima</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2491,11 +2491,11 @@
     </row>
     <row r="80">
       <c r="A80" s="15" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>orion-protocol</t>
+          <t>klondike</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2503,17 +2503,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="15" t="n">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>perpetual-protocol</t>
+          <t>kogefarm</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2521,17 +2521,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="15" t="n">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>pickle</t>
+          <t>kyber-dmm</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2539,35 +2539,35 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="15" t="n">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>pie-dao</t>
+          <t>liquity</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="15" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>pooltogether</t>
+          <t>looksrare</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2575,35 +2575,35 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="15" t="n">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>pooltogether-v4</t>
+          <t>loopring</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="15" t="n">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>popsicle</t>
+          <t>lydia</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -2617,11 +2617,11 @@
     </row>
     <row r="87">
       <c r="A87" s="15" t="n">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>powerpool</t>
+          <t>lyra</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2635,29 +2635,29 @@
     </row>
     <row r="88">
       <c r="A88" s="15" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>railgun</t>
+          <t>maker</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="15" t="n">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>rari</t>
+          <t>maple</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -2665,17 +2665,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="15" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>rari-fuse</t>
+          <t>mirror</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2689,11 +2689,11 @@
     </row>
     <row r="91">
       <c r="A91" s="15" t="n">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>redacted-cartel</t>
+          <t>mooniswap</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2701,17 +2701,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="15" t="n">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>reflexer</t>
+          <t>mstable</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2719,17 +2719,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>asset-management</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="15" t="n">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>ribbon</t>
+          <t>nexus-mutual</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2737,89 +2737,89 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="15" t="n">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>ribbon-v2</t>
+          <t>nft20</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="15" t="n">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>sablier</t>
+          <t>nftx</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="15" t="n">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>saddle</t>
+          <t>nsure-network</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="15" t="n">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>shapeshift</t>
+          <t>olympus</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="15" t="n">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>shell</t>
+          <t>ondo</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2827,17 +2827,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="15" t="n">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>snowswap</t>
+          <t>1inch</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2845,17 +2845,17 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="15" t="n">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>squid</t>
+          <t>onx</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2863,71 +2863,71 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="15" t="n">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>sushiswap</t>
+          <t>opium-network</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="15" t="n">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>sushiswap-bentobox</t>
+          <t>opyn</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="15" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>sushiswap-kashi</t>
+          <t>origin</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="15" t="n">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>swapr</t>
+          <t>orion-protocol</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2935,17 +2935,17 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="15" t="n">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>swerve</t>
+          <t>otterclam</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2953,21 +2953,21 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="15" t="n">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>synlev</t>
+          <t>pancakeswap</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2977,15 +2977,15 @@
     </row>
     <row r="107">
       <c r="A107" s="15" t="n">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>synthetix</t>
+          <t>pangolin</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2995,11 +2995,11 @@
     </row>
     <row r="108">
       <c r="A108" s="15" t="n">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>the-graph</t>
+          <t>penguin</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3007,35 +3007,35 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="15" t="n">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>tokemak</t>
+          <t>perpetual-protocol</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="15" t="n">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>tokenlon</t>
+          <t>pickle</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -3043,35 +3043,35 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>yield-aggregator</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="15" t="n">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>tornado-cash</t>
+          <t>pie-dao</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="15" t="n">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>truefi</t>
+          <t>platypus-finance</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -3079,17 +3079,17 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="15" t="n">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>unagii</t>
+          <t>polywhale</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -3103,51 +3103,51 @@
     </row>
     <row r="114">
       <c r="A114" s="15" t="n">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>uniswap</t>
+          <t>pooltogether</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>exchange</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="15" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>uniswap-v2</t>
+          <t>pooltogether-v4</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="15" t="n">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>uniswap-v3</t>
+          <t>popsicle</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -3157,11 +3157,11 @@
     </row>
     <row r="117">
       <c r="A117" s="15" t="n">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>powerpool</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3169,53 +3169,53 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="15" t="n">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>universe</t>
+          <t>qi-dao</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>lending</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="15" t="n">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>vesper</t>
+          <t>quickswap</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="15" t="n">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>wepiggy</t>
+          <t>r-u-generous</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -3223,71 +3223,71 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>lending</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="15" t="n">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>wonderland</t>
+          <t>railgun</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>exchange</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="15" t="n">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>xsigma</t>
+          <t>rari</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>liquidity-pool</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="15" t="n">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>xtoken</t>
+          <t>rari-fuse</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>liquidity-pool</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="15" t="n">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>yam</t>
+          <t>realt</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -3295,21 +3295,21 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>asset-management</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="15" t="n">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>yaxis</t>
+          <t>reaper</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3319,35 +3319,1025 @@
     </row>
     <row r="126">
       <c r="A126" s="15" t="n">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>yearn</t>
+          <t>redacted-cartel</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>yield-aggregator</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="15" t="n">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
+          <t>reflexer</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="15" t="n">
+        <v>145</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>ribbon</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>2</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="15" t="n">
+        <v>146</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>ribbon-v2</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="15" t="n">
+        <v>148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>sablier</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>2</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="15" t="n">
+        <v>149</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>saddle</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>2</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>scarecrow</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>3</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="15" t="n">
+        <v>151</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>scream</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>2</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="15" t="n">
+        <v>152</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>shapeshift</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>3</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>exchange</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="15" t="n">
+        <v>154</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>shell</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>3</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="15" t="n">
+        <v>155</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>snowball</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>3</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="15" t="n">
+        <v>156</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>snowbank</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>3</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="15" t="n">
+        <v>157</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>snowdog</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>3</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="15" t="n">
+        <v>158</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>snowswap</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>3</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="15" t="n">
+        <v>159</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>spartacus</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>3</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="15" t="n">
+        <v>160</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>spiritswap</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>2</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="15" t="n">
+        <v>161</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>spookyswap</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>2</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="15" t="n">
+        <v>162</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>squid</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>3</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="15" t="n">
+        <v>163</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>stake-dao</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="15" t="n">
+        <v>164</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>stormswap</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>3</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="15" t="n">
+        <v>165</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>superfluid</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>3</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="15" t="n">
+        <v>166</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>sushiswap</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>1</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="15" t="n">
+        <v>167</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>sushiswap-bentobox</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>1</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="15" t="n">
+        <v>168</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>sushiswap-kashi</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>1</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="15" t="n">
+        <v>169</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>swapr</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>3</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="15" t="n">
+        <v>170</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>swerve</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>3</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="15" t="n">
+        <v>171</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>synlev</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>3</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="15" t="n">
+        <v>172</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>synthetix</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>2</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="15" t="n">
+        <v>173</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>tarot</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>2</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="15" t="n">
+        <v>174</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>teddy-cash</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>3</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="15" t="n">
+        <v>175</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>the-graph</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>3</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="15" t="n">
+        <v>176</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>tokemak</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>2</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="15" t="n">
+        <v>177</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>tokenlon</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>3</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>asset-management</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="15" t="n">
+        <v>180</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>tomb</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>3</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="15" t="n">
+        <v>181</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>tornado-cash</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>2</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="15" t="n">
+        <v>182</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>traderjoe</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>1</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="15" t="n">
+        <v>184</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>truefi</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>2</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="15" t="n">
+        <v>185</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>ubeswap</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>3</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="15" t="n">
+        <v>186</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>unagii</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>3</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="15" t="n">
+        <v>187</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>uniswap</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>exchange</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="15" t="n">
+        <v>188</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>uniswap-v2</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="15" t="n">
+        <v>189</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>uniswap-v3</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>3</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="15" t="n">
+        <v>191</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>universe</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>3</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="15" t="n">
+        <v>193</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>venus</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="15" t="n">
+        <v>194</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>vesper</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>3</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="15" t="n">
+        <v>195</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>vesta-finance</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>3</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="15" t="n">
+        <v>197</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>waultswap</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>3</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="15" t="n">
+        <v>198</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>wepiggy</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>3</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>lending</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="15" t="n">
+        <v>199</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>wonderland</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>2</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>xsigma</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>3</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>liquidity-pool</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="15" t="n">
+        <v>201</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>xtoken</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>3</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>asset-management</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="15" t="n">
+        <v>202</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>yam</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>3</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>asset-management</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="15" t="n">
+        <v>203</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>yaxis</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>3</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="15" t="n">
+        <v>204</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>yearn</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="15" t="n">
+        <v>208</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
           <t>zlot</t>
         </is>
       </c>
-      <c r="C127" t="n">
-        <v>3</v>
-      </c>
-      <c r="D127" t="inlineStr">
+      <c r="C181" t="n">
+        <v>3</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>yield-aggregator</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="15" t="n">
+        <v>210</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>morpheus-swap</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>3</v>
+      </c>
+      <c r="D182" t="inlineStr">
         <is>
           <t>yield-aggregator</t>
         </is>

</xml_diff>